<commit_message>
Solve 2025, day 2
</commit_message>
<xml_diff>
--- a/2025/RuntimesChart.xlsx
+++ b/2025/RuntimesChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\efrees\adventOfCode\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC56438-335C-4FED-8776-A817453F2CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF840A8-C6ED-4820-8622-198F9A79CDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1575" windowWidth="28800" windowHeight="11295" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="9984" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -194,6 +194,9 @@
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -205,6 +208,9 @@
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2.2661199999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8892599999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1324,24 +1330,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.83984375" customWidth="1"/>
+    <col min="2" max="2" width="14.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1349,7 +1355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1357,6 +1363,14 @@
         <v>2.2661199999999999E-3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3.8892599999999999E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Solve 2025, day 3
</commit_message>
<xml_diff>
--- a/2025/RuntimesChart.xlsx
+++ b/2025/RuntimesChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\efrees\adventOfCode\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF840A8-C6ED-4820-8622-198F9A79CDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6673FCDC-5120-4C42-A20B-8613BD336C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="9984" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="-22728" yWindow="312" windowWidth="17280" windowHeight="9984" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -197,6 +197,9 @@
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -211,6 +214,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.8892599999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5803999999999995E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1330,24 +1336,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83984375" customWidth="1"/>
-    <col min="2" max="2" width="14.83984375" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1363,7 +1369,7 @@
         <v>2.2661199999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1371,6 +1377,14 @@
         <v>3.8892599999999999E-3</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>9.5803999999999995E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Solve 2025, day 4
</commit_message>
<xml_diff>
--- a/2025/RuntimesChart.xlsx
+++ b/2025/RuntimesChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\efrees\adventOfCode\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6673FCDC-5120-4C42-A20B-8613BD336C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BE1EE3-2657-4506-86A1-160C52292925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22728" yWindow="312" windowWidth="17280" windowHeight="9984" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
@@ -200,6 +200,9 @@
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -217,6 +220,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.5803999999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10504788</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1336,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,6 +1391,14 @@
         <v>9.5803999999999995E-4</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.10504788</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Solve 2025, day 5, part 2
</commit_message>
<xml_diff>
--- a/2025/RuntimesChart.xlsx
+++ b/2025/RuntimesChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\efrees\adventOfCode\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BE1EE3-2657-4506-86A1-160C52292925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D3DA4C-978F-4ED3-9A99-629E538D43FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22728" yWindow="312" windowWidth="17280" windowHeight="9984" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="16500" yWindow="2370" windowWidth="17280" windowHeight="9990" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -203,6 +203,9 @@
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -223,6 +226,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.10504788</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0531999999999998E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1342,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,6 +1405,14 @@
         <v>0.10504788</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>3.0531999999999998E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Solve 2025, day 6
</commit_message>
<xml_diff>
--- a/2025/RuntimesChart.xlsx
+++ b/2025/RuntimesChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\efrees\adventOfCode\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D3DA4C-978F-4ED3-9A99-629E538D43FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67365B2C-A56F-4668-A81E-9ABD25F4394E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="2370" windowWidth="17280" windowHeight="9990" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="17280" windowHeight="9984" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -206,6 +206,9 @@
                 <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -229,6 +232,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.0531999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8369199999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1348,24 +1354,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.83984375" customWidth="1"/>
+    <col min="2" max="2" width="14.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1381,7 +1387,7 @@
         <v>2.2661199999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>3.8892599999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>9.5803999999999995E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1405,7 +1411,7 @@
         <v>0.10504788</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1413,6 +1419,14 @@
         <v>3.0531999999999998E-3</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1.8369199999999999E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Solve 2025, day 7
</commit_message>
<xml_diff>
--- a/2025/RuntimesChart.xlsx
+++ b/2025/RuntimesChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\efrees\adventOfCode\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67365B2C-A56F-4668-A81E-9ABD25F4394E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E890665D-ED62-46C4-9B37-C6257144C4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1830" windowWidth="17280" windowHeight="9984" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="12" yWindow="156" windowWidth="23028" windowHeight="13668" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -209,6 +209,9 @@
                 <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -235,6 +238,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.8369199999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5176000000000003E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1354,24 +1360,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83984375" customWidth="1"/>
-    <col min="2" max="2" width="14.83984375" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1379,7 +1385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1387,7 +1393,7 @@
         <v>2.2661199999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1395,7 +1401,7 @@
         <v>3.8892599999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1403,7 +1409,7 @@
         <v>9.5803999999999995E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>0.10504788</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1419,12 +1425,20 @@
         <v>3.0531999999999998E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>1.8369199999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>6.5176000000000003E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solve 2025, day 8
</commit_message>
<xml_diff>
--- a/2025/RuntimesChart.xlsx
+++ b/2025/RuntimesChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\efrees\adventOfCode\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E890665D-ED62-46C4-9B37-C6257144C4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0B3CDB-938C-4B49-8ABD-BFDA75D27D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="156" windowWidth="23028" windowHeight="13668" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="11220" yWindow="870" windowWidth="23025" windowHeight="13665" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -212,6 +212,9 @@
                 <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -241,6 +244,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6.5176000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2092489999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1360,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,6 +1447,14 @@
         <v>6.5176000000000003E-4</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2.2092489999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Solve 2025, day 11
</commit_message>
<xml_diff>
--- a/2025/RuntimesChart.xlsx
+++ b/2025/RuntimesChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\efrees\adventOfCode\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0B3CDB-938C-4B49-8ABD-BFDA75D27D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9965B027-B0FD-4780-8C6E-C86A696B7084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11220" yWindow="870" windowWidth="23025" windowHeight="13665" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
@@ -215,6 +215,15 @@
                 <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -247,6 +256,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.2092489999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.6514000000000003E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1366,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,6 +1467,24 @@
         <v>2.2092489999999998</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>8.6514000000000003E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>